<commit_message>
Create a new dataset with names only
</commit_message>
<xml_diff>
--- a/Data/Sleutellijst_hix_onzedata.xlsx
+++ b/Data/Sleutellijst_hix_onzedata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\GitHub\Utilitarian-distribution-of-OR-capacity-during-COVID-19\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/Utilitarian-distribution-of-OR-capacity-during-COVID-19/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ED52E6-B603-40C8-A194-5DDEADC4F96C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0B182E-0F43-1946-81F8-DD0275FD7E3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>transabdominal repair</t>
-  </si>
-  <si>
-    <t>Carotid endarteriectomy</t>
   </si>
   <si>
     <t>Patients with symptomatic carotid artery plaques</t>
@@ -588,6 +585,9 @@
   <si>
     <t>Patients with mild laryngeal cancer</t>
   </si>
+  <si>
+    <t>Carotid endarterectomy</t>
+  </si>
 </sst>
 </file>
 
@@ -857,7 +857,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1073,20 +1073,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD811"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="37.69921875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="51.69921875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" style="13" customWidth="1"/>
     <col min="3" max="3" width="30" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="2"/>
-    <col min="5" max="16384" width="12.59765625" style="3"/>
+    <col min="4" max="4" width="12.6640625" style="2"/>
+    <col min="5" max="16384" width="12.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -1097,47 +1097,47 @@
         <v>0</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>110</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1148,29 +1148,29 @@
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>12</v>
@@ -1179,38 +1179,38 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -1221,10 +1221,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1235,13 +1235,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -1252,27 +1252,27 @@
         <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
@@ -1283,10 +1283,10 @@
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1297,10 +1297,10 @@
         <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
@@ -1322,10 +1322,10 @@
         <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>37</v>
       </c>
@@ -1347,19 +1347,19 @@
         <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -1370,10 +1370,10 @@
         <v>42</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>43</v>
       </c>
@@ -1384,334 +1384,334 @@
         <v>45</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D21" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="B22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>112</v>
       </c>
+      <c r="D33" s="15" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>82</v>
+    <row r="34" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>111</v>
+    <row r="35" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="4" t="s">
+    <row r="36" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D37" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D38" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>67</v>
+    <row r="39" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D39" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>70</v>
+    <row r="40" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D40" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>81</v>
+    <row r="41" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D41" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>96</v>
+    <row r="42" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D42" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>99</v>
+    <row r="43" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D43" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="44" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="22" t="s">
+      <c r="B44" s="18" t="s">
         <v>181</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>182</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="C45" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="D45" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>58</v>
+      <c r="B46" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="C47" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="18"/>
@@ -18094,925 +18094,925 @@
       <c r="XFC47" s="18"/>
       <c r="XFD47" s="4"/>
     </row>
-    <row r="48" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D49" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="E49" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>133</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B52" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D53" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D54" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D55" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D57" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>88</v>
+      <c r="C58" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>89</v>
+    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="4" t="s">
-        <v>93</v>
+    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D54" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="C61" s="18" t="s">
         <v>127</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>128</v>
       </c>
       <c r="D61" s="27"/>
     </row>
-    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -19026,15 +19026,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100632327FA9DD42148A9BE060DEC92123E" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="2a2ad65681c873cbdee59de209d2533a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="34341ba9-d7b5-4d76-8d27-81dc39018ef7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="059be763291617e0b351699f9afda6df" ns2:_="">
     <xsd:import namespace="34341ba9-d7b5-4d76-8d27-81dc39018ef7"/>
@@ -19166,6 +19157,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2DDD85-B311-48E3-A94D-7BCBD20ECC7E}">
   <ds:schemaRefs>
@@ -19176,14 +19176,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04A2B261-E070-4582-B105-CAD4A336EDA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E3540B8-8555-48E6-949D-757E3F0B7BDD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19199,4 +19191,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04A2B261-E070-4582-B105-CAD4A336EDA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>